<commit_message>
Fix data & job shop mip model
Data: Change index and value + add sources
MIP model: linearize max and quadratic (binary*continuous) constraints
</commit_message>
<xml_diff>
--- a/job shop/data.xlsx
+++ b/job shop/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OR_Programming\job_shop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\GitHub\Operational-Research\job shop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3D9006-A354-404A-9297-40FA7A542ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90FB4A3-9AA4-4F78-BA8C-D74B826117DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ABBC1056-6D52-4ED7-A619-93DFACFDE92C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ABBC1056-6D52-4ED7-A619-93DFACFDE92C}"/>
   </bookViews>
   <sheets>
     <sheet name="set" sheetId="1" r:id="rId1"/>
@@ -184,10 +184,436 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>583815</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171602</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6471D000-CDA0-C24D-4AB3-556EA97B382F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4579620" y="0"/>
+          <a:ext cx="6344535" cy="1086002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>219951</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>30613</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DE80CE7-CF98-BE69-4210-440A4E4DF8BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3672840" y="2004060"/>
+          <a:ext cx="6277851" cy="952633"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>191388</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>129912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5198624A-FB1E-3C23-A943-97FAD19A5FE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4556760" y="571500"/>
+          <a:ext cx="6363588" cy="2667372"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>568575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>141122</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27E0C6E8-4C56-4177-8CBF-8A5CC8728627}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2514600" y="1798320"/>
+          <a:ext cx="6344535" cy="1086002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>420063</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80417</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68F465B5-242D-AA98-6B90-CCD15D3953F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4229100" y="91440"/>
+          <a:ext cx="6897063" cy="2915057"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>576195</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>156362</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED1E7A7D-1BFA-4DA2-A8E3-660219DDEAC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2499360" y="3276600"/>
+          <a:ext cx="6344535" cy="1086002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>183843</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{459C5C32-500C-41B6-83B3-D079C601FDB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3040380" y="0"/>
+          <a:ext cx="6897063" cy="2915057"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>218077</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>36481</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABBEFB9F-3905-950E-45A8-D251ACADFE61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4693920" y="0"/>
+          <a:ext cx="6496957" cy="2048161"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>484755</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>49682</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36AC9794-82CC-44AE-8D2B-4C5A3B647184}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3284220" y="60960"/>
+          <a:ext cx="6344535" cy="1086002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -225,7 +651,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -331,7 +757,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -473,7 +899,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -483,16 +909,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531E6986-C08F-494B-965A-24BD9B37D412}">
   <dimension ref="A2:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -500,10 +926,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -514,7 +940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -525,7 +951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -536,7 +962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -544,10 +970,10 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -555,12 +981,13 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -568,17 +995,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D17A1B9-234D-48E0-A78E-38803F19F954}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -592,253 +1019,253 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -857,13 +1284,13 @@
       <selection activeCell="A2" sqref="A2:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -877,253 +1304,253 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1142,13 +1569,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1156,24 +1583,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1185,13 +1613,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1202,74 +1630,75 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>180</v>
       </c>
       <c r="C2">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>200</v>
       </c>
       <c r="C3">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
       <c r="C4">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>165</v>
       </c>
       <c r="C5">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>120</v>
       </c>
       <c r="C6">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>150</v>
       </c>
       <c r="C7">
-        <v>155</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1281,12 +1710,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1294,49 +1723,49 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>85</v>
@@ -1344,20 +1773,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10217E5-848D-408C-83F2-E067233C0550}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1373,8 +1803,11 @@
       <c r="E1">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1382,21 +1815,24 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1407,13 +1843,16 @@
       <c r="E3">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>41</v>
@@ -1424,13 +1863,16 @@
       <c r="E4">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>75</v>
@@ -1441,9 +1883,33 @@
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1455,9 +1921,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1465,32 +1931,33 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1502,13 +1969,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1519,37 +1986,37 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>190</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>